<commit_message>
data updated & ph added
</commit_message>
<xml_diff>
--- a/src/assets/AllIndicesExample.xlsx
+++ b/src/assets/AllIndicesExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\admin_vsfintech\adminpanel\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B28AFA-F470-48C9-B4C9-A8736705D856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39A4E4C-41D0-491F-941C-826689AA2726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,12 +70,6 @@
     <t>NFT500</t>
   </si>
   <si>
-    <t>GNFT500MC50:25:25</t>
-  </si>
-  <si>
-    <t>NFT500MC50:25:25</t>
-  </si>
-  <si>
     <t>GNFT500LGMSEQLCAPWTD</t>
   </si>
   <si>
@@ -358,18 +352,6 @@
     <t>NFT200QLT30</t>
   </si>
   <si>
-    <t>GNFT50SRTDURDEBTDYNP/B</t>
-  </si>
-  <si>
-    <t>NFT50SRTDURDEBTDYNP/B</t>
-  </si>
-  <si>
-    <t>GNFT50SRTDURDEBTDYNP/E</t>
-  </si>
-  <si>
-    <t>NFT50SRTDURDEBTDYNP/E</t>
-  </si>
-  <si>
     <t>GNFTEQTSAV</t>
   </si>
   <si>
@@ -457,9 +439,6 @@
     <t>NFTINDCORPGRPITG</t>
   </si>
   <si>
-    <t>NFTINDCORPGRPITG25%C</t>
-  </si>
-  <si>
     <t>NFTTRANSLOG</t>
   </si>
   <si>
@@ -472,12 +451,6 @@
     <t>NFT500SH</t>
   </si>
   <si>
-    <t>NFT500MULCINDMFG50:30:20</t>
-  </si>
-  <si>
-    <t>NFT500MULCINFS50:30:20</t>
-  </si>
-  <si>
     <t>NFTSMEEMG</t>
   </si>
   <si>
@@ -490,9 +463,6 @@
     <t>NFTFINSERV</t>
   </si>
   <si>
-    <t>NFTFINSERV25/50</t>
-  </si>
-  <si>
     <t>NFTFINSERVEB</t>
   </si>
   <si>
@@ -625,9 +595,6 @@
     <t>GNFTINDCORPGRPITG</t>
   </si>
   <si>
-    <t>GNFTINDCORPGRPITG25%C</t>
-  </si>
-  <si>
     <t>GNFTTRANSLOG</t>
   </si>
   <si>
@@ -640,12 +607,6 @@
     <t>GNFT500SH</t>
   </si>
   <si>
-    <t>GNFT500MULCINDMFG50:30:20</t>
-  </si>
-  <si>
-    <t>GNFT500MULCINFS50:30:20</t>
-  </si>
-  <si>
     <t>GNFTSMEEMG</t>
   </si>
   <si>
@@ -658,9 +619,6 @@
     <t>GNFTFINSERV</t>
   </si>
   <si>
-    <t>GNFTFINSERV25/50</t>
-  </si>
-  <si>
     <t>GNFTFINSERVEB</t>
   </si>
   <si>
@@ -716,6 +674,48 @@
   </si>
   <si>
     <t>This is PCNT</t>
+  </si>
+  <si>
+    <t>GNFT50SRTDURDEBTDYNP_B</t>
+  </si>
+  <si>
+    <t>NFT50SRTDURDEBTDYNP_B</t>
+  </si>
+  <si>
+    <t>GNFT50SRTDURDEBTDYNP_E</t>
+  </si>
+  <si>
+    <t>NFT50SRTDURDEBTDYNP_E</t>
+  </si>
+  <si>
+    <t>GNFTFINSERV25_50</t>
+  </si>
+  <si>
+    <t>NFTFINSERV25_50</t>
+  </si>
+  <si>
+    <t>GNFT500MC50_25_25</t>
+  </si>
+  <si>
+    <t>NFT500MC50_25_25</t>
+  </si>
+  <si>
+    <t>GNFT500MULCINDMFG50_30_20</t>
+  </si>
+  <si>
+    <t>NFT500MULCINDMFG50_30_20</t>
+  </si>
+  <si>
+    <t>GNFT500MULCINFS50_30_20</t>
+  </si>
+  <si>
+    <t>NFT500MULCINFS50_30_20</t>
+  </si>
+  <si>
+    <t>GNFTINDCORPGRPITG25PC</t>
+  </si>
+  <si>
+    <t>NFTINDCORPGRPITG25PC</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:HT4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1487,646 +1487,646 @@
         <v>15</v>
       </c>
       <c r="O1" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="T1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="U1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="V1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="W1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="X1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="Y1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="Z1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="23" t="s">
+      <c r="AA1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="23" t="s">
+      <c r="AB1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AC1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="23" t="s">
+      <c r="AD1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AH1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="23" t="s">
+      <c r="AI1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AK1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AL1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" s="23" t="s">
+      <c r="AM1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" s="23" t="s">
+      <c r="AN1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" s="23" t="s">
+      <c r="AO1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AN1" s="23" t="s">
+      <c r="AP1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AO1" s="23" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" s="23" t="s">
+      <c r="AR1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AQ1" s="23" t="s">
+      <c r="AS1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" s="23" t="s">
+      <c r="AT1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" s="23" t="s">
+      <c r="AU1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="AT1" s="23" t="s">
+      <c r="AV1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="AU1" s="23" t="s">
+      <c r="AW1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AV1" s="23" t="s">
+      <c r="AX1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AW1" s="23" t="s">
+      <c r="AY1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AX1" s="23" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AY1" s="23" t="s">
+      <c r="BA1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AZ1" s="23" t="s">
+      <c r="BB1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="BA1" s="23" t="s">
+      <c r="BC1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="BB1" s="23" t="s">
+      <c r="BD1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" s="23" t="s">
+      <c r="BE1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="BD1" s="23" t="s">
+      <c r="BF1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="BE1" s="23" t="s">
+      <c r="BG1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="BF1" s="23" t="s">
+      <c r="BH1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="BG1" s="23" t="s">
+      <c r="BI1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="BH1" s="23" t="s">
+      <c r="BJ1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BI1" s="23" t="s">
+      <c r="BK1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="BJ1" s="23" t="s">
+      <c r="BL1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BK1" s="23" t="s">
+      <c r="BM1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BL1" s="23" t="s">
+      <c r="BN1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BM1" s="23" t="s">
+      <c r="BO1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BN1" s="23" t="s">
+      <c r="BP1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="BO1" s="23" t="s">
+      <c r="BQ1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="BP1" s="23" t="s">
+      <c r="BR1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="BQ1" s="23" t="s">
+      <c r="BS1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="BR1" s="23" t="s">
+      <c r="BT1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="BS1" s="23" t="s">
+      <c r="BU1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="BT1" s="23" t="s">
+      <c r="BV1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="BU1" s="23" t="s">
+      <c r="BW1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="BV1" s="23" t="s">
+      <c r="BX1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="BW1" s="23" t="s">
+      <c r="BY1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="BX1" s="23" t="s">
+      <c r="BZ1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="BY1" s="23" t="s">
+      <c r="CA1" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="BZ1" s="23" t="s">
+      <c r="CB1" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="CA1" s="23" t="s">
+      <c r="CC1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="CB1" s="23" t="s">
+      <c r="CD1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="CC1" s="23" t="s">
+      <c r="CE1" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="CD1" s="23" t="s">
+      <c r="CF1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="CE1" s="23" t="s">
+      <c r="CG1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="CF1" s="23" t="s">
+      <c r="CH1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="CG1" s="23" t="s">
+      <c r="CI1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="CH1" s="23" t="s">
+      <c r="CJ1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="CI1" s="23" t="s">
+      <c r="CK1" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="CJ1" s="23" t="s">
+      <c r="CL1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="CK1" s="23" t="s">
+      <c r="CM1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="CL1" s="23" t="s">
+      <c r="CN1" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="CM1" s="23" t="s">
+      <c r="CO1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="CN1" s="23" t="s">
+      <c r="CP1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="CO1" s="23" t="s">
+      <c r="CQ1" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="CP1" s="23" t="s">
+      <c r="CR1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="CQ1" s="23" t="s">
+      <c r="CS1" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="CR1" s="23" t="s">
+      <c r="CT1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="CS1" s="23" t="s">
+      <c r="CU1" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="CT1" s="23" t="s">
+      <c r="CV1" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="CU1" s="23" t="s">
+      <c r="CW1" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="CV1" s="23" t="s">
+      <c r="CX1" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="CW1" s="23" t="s">
+      <c r="CY1" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="CX1" s="23" t="s">
+      <c r="CZ1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="CY1" s="23" t="s">
+      <c r="DA1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="CZ1" s="23" t="s">
+      <c r="DB1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="DA1" s="23" t="s">
+      <c r="DC1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="DB1" s="23" t="s">
+      <c r="DD1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="DC1" s="23" t="s">
+      <c r="DE1" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="DD1" s="23" t="s">
+      <c r="DF1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="DE1" s="23" t="s">
+      <c r="DG1" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="DH1" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="DI1" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="DJ1" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="DK1" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="DF1" s="23" t="s">
+      <c r="DL1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="DG1" s="23" t="s">
+      <c r="DM1" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="DN1" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="DH1" s="23" t="s">
+      <c r="DO1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="DP1" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="DI1" s="23" t="s">
+      <c r="DQ1" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="DR1" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="DJ1" s="23" t="s">
+      <c r="DS1" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="DT1" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="DK1" s="23" t="s">
+      <c r="DU1" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="DV1" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="DL1" s="23" t="s">
+      <c r="DW1" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="DX1" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="DM1" s="23" t="s">
+      <c r="DY1" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="DZ1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="EA1" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="EB1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="EC1" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="ED1" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="EE1" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="EF1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="EG1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="DN1" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="DO1" s="23" t="s">
+      <c r="EH1" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="EI1" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="DP1" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="DQ1" s="23" t="s">
+      <c r="EJ1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="EK1" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="DR1" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="DS1" s="24" t="s">
+      <c r="EL1" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="EM1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="DT1" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="DU1" s="23" t="s">
+      <c r="EN1" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="EO1" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="DV1" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="DW1" s="23" t="s">
+      <c r="EP1" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="EQ1" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="DX1" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="DY1" s="23" t="s">
+      <c r="ER1" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="ES1" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="DZ1" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="EA1" s="23" t="s">
+      <c r="ET1" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="EU1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="EB1" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="EC1" s="23" t="s">
+      <c r="EV1" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="EW1" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="ED1" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="EE1" s="23" t="s">
+      <c r="EX1" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="EY1" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="EF1" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="EG1" s="23" t="s">
+      <c r="EZ1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="FA1" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="EH1" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="EI1" s="23" t="s">
+      <c r="FB1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="FC1" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="EJ1" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="EK1" s="23" t="s">
+      <c r="FD1" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="FE1" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="EL1" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="EM1" s="23" t="s">
+      <c r="FF1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="FG1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="EN1" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="EO1" s="23" t="s">
+      <c r="FH1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="FI1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="EP1" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="EQ1" s="24" t="s">
+      <c r="FJ1" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="FK1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="ER1" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="ES1" s="23" t="s">
+      <c r="FL1" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="FM1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="ET1" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="EU1" s="23" t="s">
+      <c r="FN1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="FO1" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="FP1" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="FQ1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="EV1" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="EW1" s="23" t="s">
+      <c r="FR1" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="FS1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="EX1" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="EY1" s="23" t="s">
+      <c r="FT1" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="FU1" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="EZ1" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="FA1" s="23" t="s">
+      <c r="FV1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="FW1" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="FB1" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="FC1" s="23" t="s">
+      <c r="FX1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="FY1" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="FZ1" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="GA1" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="GB1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="GC1" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="FD1" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="FE1" s="23" t="s">
+      <c r="GD1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="GE1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="FF1" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="FG1" s="23" t="s">
+      <c r="GF1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="GG1" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="FH1" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="FI1" s="23" t="s">
+      <c r="GH1" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="GI1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="FJ1" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="FK1" s="23" t="s">
+      <c r="GJ1" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="GK1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="GL1" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="GM1" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="FL1" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="FM1" s="23" t="s">
+      <c r="GN1" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="GO1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="FN1" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="FO1" s="23" t="s">
+      <c r="GP1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="GQ1" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="FP1" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="FQ1" s="23" t="s">
+      <c r="GR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="GS1" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="FR1" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="FS1" s="23" t="s">
+      <c r="GT1" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="GU1" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="FT1" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="FU1" s="23" t="s">
+      <c r="GV1" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="GW1" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="FV1" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="FW1" s="23" t="s">
+      <c r="GX1" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="GY1" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="FX1" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="FY1" s="23" t="s">
+      <c r="GZ1" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="HA1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="FZ1" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="GA1" s="24" t="s">
+      <c r="HB1" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="HC1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="GB1" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="GC1" s="23" t="s">
+      <c r="HD1" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="HE1" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="GD1" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="GE1" s="23" t="s">
+      <c r="HF1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="HG1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="GF1" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="GG1" s="23" t="s">
+      <c r="HH1" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="HI1" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="GH1" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="GI1" s="23" t="s">
+      <c r="HJ1" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="HK1" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="GJ1" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="GK1" s="23" t="s">
+      <c r="HL1" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="HM1" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="GL1" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="GM1" s="23" t="s">
+      <c r="HN1" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="HO1" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="GN1" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="GO1" s="23" t="s">
+      <c r="HP1" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="HQ1" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="GP1" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="GQ1" s="23" t="s">
+      <c r="HR1" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="HS1" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="GR1" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="GS1" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="GT1" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="GU1" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="GV1" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="GW1" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="GX1" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="GY1" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="GZ1" s="23" t="s">
+      <c r="HT1" s="23" t="s">
         <v>163</v>
-      </c>
-      <c r="HA1" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="HB1" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="HC1" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="HD1" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="HE1" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="HF1" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="HG1" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="HH1" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="HI1" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="HJ1" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="HK1" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="HL1" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="HM1" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="HN1" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="HO1" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="HP1" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="HQ1" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="HR1" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="HS1" s="23" t="s">
-        <v>229</v>
-      </c>
-      <c r="HT1" s="23" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:228" ht="14.4">
@@ -2660,6 +2660,156 @@
       <c r="FV2" s="3">
         <v>0.1</v>
       </c>
+      <c r="FW2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="FX2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="FY2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="FZ2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GA2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GB2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GC2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GD2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GE2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GF2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GG2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GH2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GI2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GJ2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GK2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GL2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GM2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GN2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GO2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GP2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GQ2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GR2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GS2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GT2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GU2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GV2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GW2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GX2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="GY2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="GZ2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HA2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HB2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HC2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HD2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HE2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HF2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HG2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HH2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HI2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HJ2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HK2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HL2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HM2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HN2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HO2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HP2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HQ2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HR2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="HS2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="HT2" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3" spans="1:228" ht="43.2">
       <c r="A3" s="4" t="s">
@@ -2669,10 +2819,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
@@ -2848,6 +2998,56 @@
       <c r="FT3" s="6"/>
       <c r="FU3" s="6"/>
       <c r="FV3" s="6"/>
+      <c r="FW3" s="6"/>
+      <c r="FX3" s="6"/>
+      <c r="FY3" s="6"/>
+      <c r="FZ3" s="6"/>
+      <c r="GA3" s="6"/>
+      <c r="GB3" s="6"/>
+      <c r="GC3" s="6"/>
+      <c r="GD3" s="6"/>
+      <c r="GE3" s="6"/>
+      <c r="GF3" s="6"/>
+      <c r="GG3" s="6"/>
+      <c r="GH3" s="6"/>
+      <c r="GI3" s="6"/>
+      <c r="GJ3" s="6"/>
+      <c r="GK3" s="6"/>
+      <c r="GL3" s="6"/>
+      <c r="GM3" s="6"/>
+      <c r="GN3" s="6"/>
+      <c r="GO3" s="6"/>
+      <c r="GP3" s="6"/>
+      <c r="GQ3" s="6"/>
+      <c r="GR3" s="6"/>
+      <c r="GS3" s="6"/>
+      <c r="GT3" s="6"/>
+      <c r="GU3" s="6"/>
+      <c r="GV3" s="6"/>
+      <c r="GW3" s="6"/>
+      <c r="GX3" s="6"/>
+      <c r="GY3" s="6"/>
+      <c r="GZ3" s="6"/>
+      <c r="HA3" s="6"/>
+      <c r="HB3" s="6"/>
+      <c r="HC3" s="6"/>
+      <c r="HD3" s="6"/>
+      <c r="HE3" s="6"/>
+      <c r="HF3" s="6"/>
+      <c r="HG3" s="6"/>
+      <c r="HH3" s="6"/>
+      <c r="HI3" s="6"/>
+      <c r="HJ3" s="6"/>
+      <c r="HK3" s="6"/>
+      <c r="HL3" s="6"/>
+      <c r="HM3" s="6"/>
+      <c r="HN3" s="6"/>
+      <c r="HO3" s="6"/>
+      <c r="HP3" s="6"/>
+      <c r="HQ3" s="6"/>
+      <c r="HR3" s="6"/>
+      <c r="HS3" s="6"/>
+      <c r="HT3" s="6"/>
     </row>
     <row r="4" spans="1:228" ht="14.4">
       <c r="A4" s="10"/>

</xml_diff>